<commit_message>
v Encore un jour
</commit_message>
<xml_diff>
--- a/Duolingo.xlsx
+++ b/Duolingo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github.com\Punkyherisson\MinnaNoNihongo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github.com\Punkyherisson\MinnaNoNihongo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C699FF-1D7B-480A-BA4B-868624E591F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A817ECE-6FDB-45EF-9638-015CAD629DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3957BE59-76E7-45D0-89F8-36C2D1B53CE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>tokidoki hon o yomimasuka</t>
   </si>
@@ -254,10 +254,58 @@
     <t>tv and movies</t>
   </si>
   <si>
-    <t>Romaji</t>
-  </si>
-  <si>
-    <t>Japanese</t>
+    <t>romaji</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>basukettoboru o shimasuka</t>
+  </si>
+  <si>
+    <t>hai terebi o mimasu</t>
+  </si>
+  <si>
+    <t>yes i watch tv</t>
+  </si>
+  <si>
+    <t>hon o yo mimasuka</t>
+  </si>
+  <si>
+    <t>do you read books</t>
+  </si>
+  <si>
+    <t>jpoppu okikimasuka</t>
+  </si>
+  <si>
+    <t>do you listen to jpop</t>
+  </si>
+  <si>
+    <t>yoku hon o yomimasu</t>
+  </si>
+  <si>
+    <t>i often read books</t>
+  </si>
+  <si>
+    <t>ongaku o kikimasuka</t>
+  </si>
+  <si>
+    <t>do you listen to music</t>
+  </si>
+  <si>
+    <t>yakyu u o shimasu</t>
+  </si>
+  <si>
+    <t>i play baseball</t>
+  </si>
+  <si>
+    <t>yoku eiga o mimasuka</t>
+  </si>
+  <si>
+    <t>do you often watch movies</t>
+  </si>
+  <si>
+    <t>naomisanwatokidokianimeomimasu</t>
   </si>
 </sst>
 </file>
@@ -273,12 +321,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -293,8 +347,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,7 +368,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,44 +684,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF8F51A-A511-48D9-A611-B24EF2100BDF}">
-  <dimension ref="F3:G39"/>
+  <dimension ref="F3:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -674,266 +729,335 @@
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="G36" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G39" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V0.16 MAJ 22 Avril
</commit_message>
<xml_diff>
--- a/Duolingo.xlsx
+++ b/Duolingo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github.com\Punkyherisson\MinnaNoNihongo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github.com\Punkyherisson\MinnaNoNihongo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C699FF-1D7B-480A-BA4B-868624E591F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A817ECE-6FDB-45EF-9638-015CAD629DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3957BE59-76E7-45D0-89F8-36C2D1B53CE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>tokidoki hon o yomimasuka</t>
   </si>
@@ -254,10 +254,58 @@
     <t>tv and movies</t>
   </si>
   <si>
-    <t>Romaji</t>
-  </si>
-  <si>
-    <t>Japanese</t>
+    <t>romaji</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>basukettoboru o shimasuka</t>
+  </si>
+  <si>
+    <t>hai terebi o mimasu</t>
+  </si>
+  <si>
+    <t>yes i watch tv</t>
+  </si>
+  <si>
+    <t>hon o yo mimasuka</t>
+  </si>
+  <si>
+    <t>do you read books</t>
+  </si>
+  <si>
+    <t>jpoppu okikimasuka</t>
+  </si>
+  <si>
+    <t>do you listen to jpop</t>
+  </si>
+  <si>
+    <t>yoku hon o yomimasu</t>
+  </si>
+  <si>
+    <t>i often read books</t>
+  </si>
+  <si>
+    <t>ongaku o kikimasuka</t>
+  </si>
+  <si>
+    <t>do you listen to music</t>
+  </si>
+  <si>
+    <t>yakyu u o shimasu</t>
+  </si>
+  <si>
+    <t>i play baseball</t>
+  </si>
+  <si>
+    <t>yoku eiga o mimasuka</t>
+  </si>
+  <si>
+    <t>do you often watch movies</t>
+  </si>
+  <si>
+    <t>naomisanwatokidokianimeomimasu</t>
   </si>
 </sst>
 </file>
@@ -273,12 +321,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -293,8 +347,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,7 +368,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,44 +684,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF8F51A-A511-48D9-A611-B24EF2100BDF}">
-  <dimension ref="F3:G39"/>
+  <dimension ref="F3:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -674,266 +729,335 @@
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="G36" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G39" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>